<commit_message>
add filter in export excell
</commit_message>
<xml_diff>
--- a/kasus.xlsx
+++ b/kasus.xlsx
@@ -14,110 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34" count="34">
-  <x:si>
-    <x:t>ID Kasus</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NIK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nama</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tanggal Lahir</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Usia</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jenis Kelamin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Alamat Tempat Tinggal</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kewarganegaraan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No. Telp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pekerjaan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Status</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tahapan</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hasil</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lokasi saat ini</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tanggal Awal gejala</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gejala</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Riwayat</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tanggal Input</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Author</x:t>
-  </x:si>
-  <x:si>
-    <x:t>covid-1025200020</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
-  </x:si>
-  <x:si>
-    <x:t>depa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wed Jan 01 2020 00:00:00 GMT+0000 (Coordinated Universal Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>L</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ad KOTA BANJAR Banjar Banjar</x:t>
-  </x:si>
-  <x:si>
-    <x:t>WNI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>OTG</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RS IBU DAN ANAK KENARI GRAHA MEDIKA</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mon Apr 04 2016 00:00:00 GMT+0000 (Coordinated Universal Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Suhu tubuh &gt;= 38 °C,Suhu tubuh &lt; 38 °C</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wed Apr 08 2020 09:14:05 GMT+0000 (Coordinated Universal Time)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dinkes Kota Banjar</x:t>
-  </x:si>
-</x:sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,121 +375,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:19">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="E1" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="F1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G1" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I1" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="J1" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="K1" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="L1" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="M1" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="N1" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="O1" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="P1" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="Q1" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="R1" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="S1" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:19">
-      <x:c r="A2" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="n">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="J2" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="K2" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="L2" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="M2" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="N2" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="O2" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="P2" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="Q2" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="R2" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="S2" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-    </x:row>
+    <x:row r="1" spans="1:0"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
fix count positif, meninggal and sembuh
</commit_message>
<xml_diff>
--- a/kasus.xlsx
+++ b/kasus.xlsx
@@ -14,7 +14,107 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32" count="32">
+  <x:si>
+    <x:t>ID Kasus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NIK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nama</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tanggal Lahir</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Usia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jenis Kelamin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alamat Tempat Tinggal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kewarganegaraan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No. Telp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pekerjaan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tahapan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hasil</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lokasi saat ini</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tanggal Awal gejala</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gejala</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Riwayat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tanggal Input</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Author</x:t>
+  </x:si>
+  <x:si>
+    <x:t>covid-1024200001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Liu Xiamei</x:t>
+  </x:si>
+  <x:si>
+    <x:t>L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mess PT Sansan Melong Asih KOTA CIMAHI Kelurahan Cimahi Selatan Kecamatan Cimahi Selatan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WNA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PT Sansan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ODP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MENINGGAL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mess PT Sansan Melong Asih</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24/3/2020</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>SEMBUH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dinkes Kota Cimahi</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,7 +475,115 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:0"/>
+    <x:row r="1" spans="1:19">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="L1" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="M1" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="N1" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="O1" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="Q1" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="R1" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="S1" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:19">
+      <x:c r="A2" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="Q2" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="R2" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="S2" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>